<commit_message>
made battery module optional and changed error handling in smoothing rule.
</commit_message>
<xml_diff>
--- a/models/rps/summary_costs_all_scenarios.xlsx
+++ b/models/rps/summary_costs_all_scenarios.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="20" windowWidth="29180" windowHeight="17760" tabRatio="500"/>
+    <workbookView xWindow="960" yWindow="960" windowWidth="24120" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary_all_scenarios.tsv" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="169">
   <si>
     <t>scenario</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>100% renewable by 2045 (not 2030)</t>
+  </si>
+  <si>
+    <t>no new renewables</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -762,8 +765,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -784,8 +791,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="157">
     <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Currency" xfId="33" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -863,6 +873,8 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -938,10 +950,17 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF808080"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1140,11 +1159,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2012411240"/>
-        <c:axId val="-2012339320"/>
+        <c:axId val="-2035841928"/>
+        <c:axId val="1763322632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2012411240"/>
+        <c:axId val="-2035841928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1189,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2012339320"/>
+        <c:crossAx val="1763322632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1178,7 +1197,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2012339320"/>
+        <c:axId val="1763322632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1214,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2012411240"/>
+        <c:crossAx val="-2035841928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1421,11 +1440,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2072917112"/>
-        <c:axId val="2116660184"/>
+        <c:axId val="1764943608"/>
+        <c:axId val="1755882040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2072917112"/>
+        <c:axId val="1764943608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2116660184"/>
+        <c:crossAx val="1755882040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1459,7 +1478,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2116660184"/>
+        <c:axId val="1755882040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,7 +1495,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2072917112"/>
+        <c:crossAx val="1764943608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1588,11 +1607,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2031980904"/>
-        <c:axId val="2031337640"/>
+        <c:axId val="-2021714312"/>
+        <c:axId val="-2029694536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2031980904"/>
+        <c:axId val="-2021714312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1618,7 +1637,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2031337640"/>
+        <c:crossAx val="-2029694536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1626,7 +1645,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2031337640"/>
+        <c:axId val="-2029694536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1670,7 +1689,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2031980904"/>
+        <c:crossAx val="-2021714312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1788,11 +1807,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2078814920"/>
-        <c:axId val="-2063488200"/>
+        <c:axId val="1787097224"/>
+        <c:axId val="-2031994392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2078814920"/>
+        <c:axId val="1787097224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,7 +1837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2063488200"/>
+        <c:crossAx val="-2031994392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1826,7 +1845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2063488200"/>
+        <c:axId val="-2031994392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -1870,7 +1889,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2078814920"/>
+        <c:crossAx val="1787097224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1982,11 +2001,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2073894040"/>
-        <c:axId val="-2065535288"/>
+        <c:axId val="1762261352"/>
+        <c:axId val="1752363816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2073894040"/>
+        <c:axId val="1762261352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,7 +2031,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2065535288"/>
+        <c:crossAx val="1752363816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2020,7 +2039,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2065535288"/>
+        <c:axId val="1752363816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2064,7 +2083,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2073894040"/>
+        <c:crossAx val="1762261352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2170,11 +2189,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2082560648"/>
-        <c:axId val="-2072010504"/>
+        <c:axId val="1767277272"/>
+        <c:axId val="1797961544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2082560648"/>
+        <c:axId val="1767277272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2219,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072010504"/>
+        <c:crossAx val="1797961544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2208,7 +2227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072010504"/>
+        <c:axId val="1797961544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2252,7 +2271,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="-2082560648"/>
+        <c:crossAx val="1767277272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2370,11 +2389,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2117669160"/>
-        <c:axId val="2096508808"/>
+        <c:axId val="-2028736280"/>
+        <c:axId val="2100842536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2117669160"/>
+        <c:axId val="-2028736280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2400,7 +2419,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2096508808"/>
+        <c:crossAx val="2100842536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2408,7 +2427,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2096508808"/>
+        <c:axId val="2100842536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2452,7 +2471,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2117669160"/>
+        <c:crossAx val="-2028736280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2558,11 +2577,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2097103416"/>
-        <c:axId val="2097106584"/>
+        <c:axId val="1765455368"/>
+        <c:axId val="2075474024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2097103416"/>
+        <c:axId val="1765455368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,7 +2607,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2097106584"/>
+        <c:crossAx val="2075474024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2596,7 +2615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2097106584"/>
+        <c:axId val="2075474024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2640,7 +2659,222 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2097103416"/>
+        <c:crossAx val="1765455368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1400"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="008000"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>summary_all_scenarios.tsv!$N$57:$N$61</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>no new renewables</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25% biofuel,_x000d_no demand response</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19% biofuel,_x000d_demand response</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5% biofuel,_x000d_demand response</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5% biofuel,_x000d_demand response_x000d_hydrogen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>summary_all_scenarios.tsv!$H$57:$H$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.178</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1766140488"/>
+        <c:axId val="2137728472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1766140488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2137728472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2137728472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Electricity Cost ($/kWh)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0"/>
+              <c:y val="0.192144019707034"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="1766140488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2927,6 +3161,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3259,8 +3525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5494,18 +5760,54 @@
       <c r="O56" s="11"/>
     </row>
     <row r="57" spans="1:15">
+      <c r="H57">
+        <v>0.15</v>
+      </c>
+      <c r="N57" t="s">
+        <v>168</v>
+      </c>
       <c r="O57" s="11"/>
     </row>
     <row r="58" spans="1:15">
+      <c r="H58">
+        <v>0.19</v>
+      </c>
+      <c r="N58" t="str">
+        <f>"25% biofuel,"&amp;CHAR(13)&amp;"no demand response"</f>
+        <v>25% biofuel,_x000D_no demand response</v>
+      </c>
       <c r="O58" s="11"/>
     </row>
     <row r="59" spans="1:15">
+      <c r="H59">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="N59" t="str">
+        <f>"19% biofuel,"&amp;CHAR(13)&amp;"demand response"</f>
+        <v>19% biofuel,_x000D_demand response</v>
+      </c>
       <c r="O59" s="11"/>
     </row>
     <row r="60" spans="1:15">
+      <c r="H60">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="N60" t="str">
+        <f>"5% biofuel,"&amp;CHAR(13)&amp;"demand response"</f>
+        <v>5% biofuel,_x000D_demand response</v>
+      </c>
       <c r="O60" s="11"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" ht="30">
+      <c r="H61">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="N61" s="12" t="str">
+        <f>"5% biofuel,
+demand response
+hydrogen"</f>
+        <v>5% biofuel,_x000D_demand response_x000D_hydrogen</v>
+      </c>
       <c r="O61" s="11"/>
     </row>
     <row r="62" spans="1:15">

</xml_diff>